<commit_message>
speedtrans v3 plus ,ailer
Former-commit-id: b9bc51112e8078330b5296a7c9122055e1e12486
</commit_message>
<xml_diff>
--- a/db/dummydata/st_trucking_hamburg_port.xlsx
+++ b/db/dummydata/st_trucking_hamburg_port.xlsx
@@ -16,16 +16,91 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="105">
   <si>
+    <t>City</t>
+  </si>
+  <si>
     <t>ZONE</t>
   </si>
   <si>
+    <t>FEE</t>
+  </si>
+  <si>
     <t>Zipcode</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>rate_basis</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>load_type</t>
+  </si>
+  <si>
+    <t>Courier</t>
+  </si>
+  <si>
+    <t>cargo_class</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>truck_type</t>
+  </si>
+  <si>
+    <t>cbm_ratio</t>
+  </si>
+  <si>
+    <t>load_meterage_ratio</t>
+  </si>
+  <si>
+    <t>MOT</t>
+  </si>
+  <si>
+    <t>FEE_CODE</t>
+  </si>
+  <si>
+    <t>TRUCK_TYPE</t>
+  </si>
+  <si>
+    <t>DIRECTION</t>
+  </si>
+  <si>
+    <t>CURRENCY</t>
+  </si>
+  <si>
+    <t>RATE_BASIS</t>
+  </si>
+  <si>
+    <t>TON</t>
+  </si>
+  <si>
+    <t>CBM</t>
+  </si>
+  <si>
+    <t>KG</t>
   </si>
   <si>
     <t>PROVINCE</t>
   </si>
   <si>
     <t>COUNTRY_CODE</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>SHIPMENT</t>
+  </si>
+  <si>
+    <t>BILL</t>
   </si>
   <si>
     <t>01000 - 03999</t>
@@ -88,10 +163,19 @@
     <t>66000 - 66999</t>
   </si>
   <si>
-    <t>City</t>
+    <t>CONTAINER</t>
   </si>
   <si>
-    <t>FEE</t>
+    <t>MINIMUM</t>
+  </si>
+  <si>
+    <t>WM</t>
+  </si>
+  <si>
+    <t>PERCENTAGE</t>
+  </si>
+  <si>
+    <t>load_meterage_limit</t>
   </si>
   <si>
     <t>67000 - 69999</t>
@@ -133,90 +217,6 @@
     <t>98000 - 99999</t>
   </si>
   <si>
-    <t>MOT</t>
-  </si>
-  <si>
-    <t>FEE_CODE</t>
-  </si>
-  <si>
-    <t>TRUCK_TYPE</t>
-  </si>
-  <si>
-    <t>DIRECTION</t>
-  </si>
-  <si>
-    <t>CURRENCY</t>
-  </si>
-  <si>
-    <t>RATE_BASIS</t>
-  </si>
-  <si>
-    <t>TON</t>
-  </si>
-  <si>
-    <t>CBM</t>
-  </si>
-  <si>
-    <t>KG</t>
-  </si>
-  <si>
-    <t>ITEM</t>
-  </si>
-  <si>
-    <t>SHIPMENT</t>
-  </si>
-  <si>
-    <t>BILL</t>
-  </si>
-  <si>
-    <t>CONTAINER</t>
-  </si>
-  <si>
-    <t>MINIMUM</t>
-  </si>
-  <si>
-    <t>WM</t>
-  </si>
-  <si>
-    <t>PERCENTAGE</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Scale</t>
-  </si>
-  <si>
-    <t>rate_basis</t>
-  </si>
-  <si>
-    <t>Base</t>
-  </si>
-  <si>
-    <t>load_type</t>
-  </si>
-  <si>
-    <t>Courier</t>
-  </si>
-  <si>
-    <t>cargo_class</t>
-  </si>
-  <si>
-    <t>direction</t>
-  </si>
-  <si>
-    <t>truck_type</t>
-  </si>
-  <si>
-    <t>cbm_ratio</t>
-  </si>
-  <si>
-    <t>load_meterage_ratio</t>
-  </si>
-  <si>
-    <t>load_meterage_limit</t>
-  </si>
-  <si>
     <t>Hamburg</t>
   </si>
   <si>
@@ -226,7 +226,7 @@
     <t>kg</t>
   </si>
   <si>
-    <t>PER_KG</t>
+    <t>PER_ITEM</t>
   </si>
   <si>
     <t>cargo_item</t>
@@ -344,12 +344,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <b/>
       <sz val="11.0"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <b/>
       <sz val="10.0"/>
@@ -357,11 +357,11 @@
     </font>
     <font>
       <sz val="11.0"/>
-      <name val="Arial"/>
+      <name val="Cambria"/>
     </font>
     <font>
       <sz val="11.0"/>
-      <name val="Cambria"/>
+      <name val="Arial"/>
     </font>
     <font>
       <i/>
@@ -465,46 +465,46 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="2" fillId="3" fontId="7" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="3" fontId="7" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="top"/>
@@ -521,7 +521,7 @@
     <xf borderId="4" fillId="3" fontId="7" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -600,368 +600,368 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2">
         <v>1.0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3">
         <v>2.0</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
+      <c r="C3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4">
         <v>3.0</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
+      <c r="C4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5">
         <v>4.0</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6">
         <v>5.0</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>5</v>
+      <c r="C6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7">
         <v>6.0</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
+      <c r="C7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8">
         <v>7.0</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
+      <c r="C8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9">
         <v>8.0</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
+      <c r="C9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10">
         <v>9.0</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>5</v>
+      <c r="C10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11">
         <v>10.0</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>5</v>
+      <c r="C11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12">
         <v>11.0</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>5</v>
+      <c r="C12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13">
         <v>12.0</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>5</v>
+      <c r="C13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14">
         <v>13.0</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>5</v>
+      <c r="C14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15">
         <v>14.0</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>5</v>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16">
         <v>15.0</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>5</v>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17">
         <v>16.0</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>5</v>
+      <c r="C17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18">
         <v>17.0</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>5</v>
+      <c r="C18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19">
         <v>18.0</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>5</v>
+      <c r="C19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20">
         <v>19.0</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>5</v>
+      <c r="C20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21">
         <v>20.0</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>5</v>
+      <c r="C21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22">
         <v>21.0</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>5</v>
+      <c r="C22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23">
         <v>22.0</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>5</v>
+      <c r="C23" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24">
         <v>23.0</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>5</v>
+      <c r="C24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25">
         <v>24.0</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26">
         <v>25.0</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>5</v>
+      <c r="C26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27">
         <v>26.0</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>5</v>
+      <c r="C27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28">
         <v>27.0</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>5</v>
+      <c r="C28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29">
         <v>28.0</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>5</v>
+      <c r="C29" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30">
         <v>29.0</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>5</v>
+      <c r="C30" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31">
         <v>30.0</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>5</v>
+      <c r="C31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32">
         <v>31.0</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>5</v>
+      <c r="C32" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33">
         <v>32.0</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>5</v>
+      <c r="C33" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1"/>
@@ -977,7 +977,7 @@
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1"/>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="B46" s="2"/>
+      <c r="B46" s="6"/>
     </row>
     <row r="47" ht="15.75" customHeight="1"/>
     <row r="48" ht="15.75" customHeight="1"/>
@@ -987,10 +987,10 @@
     <row r="52" ht="15.75" customHeight="1"/>
     <row r="53" ht="15.75" customHeight="1"/>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="B54" s="2"/>
+      <c r="B54" s="6"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="B55" s="2"/>
+      <c r="B55" s="6"/>
     </row>
     <row r="56" ht="15.75" customHeight="1"/>
     <row r="57" ht="15.75" customHeight="1"/>
@@ -1964,94 +1964,94 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
     </row>
     <row r="3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -3067,92 +3067,92 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="12">
         <v>1.0</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="11">
         <v>200.0</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="13">
         <v>1000.0</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="13">
         <v>130.0</v>
       </c>
       <c r="N2" s="3"/>
@@ -3162,100 +3162,100 @@
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
-      <c r="U2" s="7"/>
+      <c r="U2" s="10"/>
     </row>
     <row r="3">
-      <c r="A3" s="11"/>
-      <c r="C3" s="12" t="s">
+      <c r="A3" s="7"/>
+      <c r="C3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="V3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="W3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="Y3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="Z3" s="12" t="s">
+      <c r="Z3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AA3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="AB3" s="12" t="s">
+      <c r="AB3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="AC3" s="12" t="s">
+      <c r="AC3" s="14" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="s">
-        <v>0</v>
+      <c r="A4" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="15" t="s">
         <v>77</v>
       </c>
       <c r="D4" s="16" t="s">
@@ -3267,16 +3267,16 @@
       <c r="F4" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="15" t="s">
         <v>82</v>
       </c>
       <c r="I4" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="15" t="s">
         <v>84</v>
       </c>
       <c r="K4" s="16" t="s">
@@ -3297,7 +3297,7 @@
       <c r="P4" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" s="15" t="s">
         <v>91</v>
       </c>
       <c r="R4" s="18" t="s">
@@ -3306,7 +3306,7 @@
       <c r="S4" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="T4" s="14" t="s">
+      <c r="T4" s="15" t="s">
         <v>94</v>
       </c>
       <c r="U4" s="19" t="s">
@@ -3338,7 +3338,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B5" s="21">
@@ -3427,7 +3427,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11">
+      <c r="A6" s="7">
         <v>1.0</v>
       </c>
       <c r="B6" s="21">
@@ -3516,7 +3516,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11">
+      <c r="A7" s="7">
         <v>2.0</v>
       </c>
       <c r="B7" s="21">
@@ -3605,7 +3605,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="11">
+      <c r="A8" s="7">
         <v>3.0</v>
       </c>
       <c r="B8" s="21">
@@ -3694,7 +3694,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11">
+      <c r="A9" s="7">
         <v>4.0</v>
       </c>
       <c r="B9" s="21">
@@ -3783,7 +3783,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="11">
+      <c r="A10" s="7">
         <v>5.0</v>
       </c>
       <c r="B10" s="21">
@@ -3872,7 +3872,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11">
+      <c r="A11" s="7">
         <v>6.0</v>
       </c>
       <c r="B11" s="21">
@@ -3961,7 +3961,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="11">
+      <c r="A12" s="7">
         <v>7.0</v>
       </c>
       <c r="B12" s="21">
@@ -4050,7 +4050,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11">
+      <c r="A13" s="7">
         <v>8.0</v>
       </c>
       <c r="B13" s="21">
@@ -4139,7 +4139,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="11">
+      <c r="A14" s="7">
         <v>9.0</v>
       </c>
       <c r="B14" s="21">
@@ -4228,7 +4228,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11">
+      <c r="A15" s="7">
         <v>10.0</v>
       </c>
       <c r="B15" s="21">
@@ -4317,7 +4317,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="11">
+      <c r="A16" s="7">
         <v>11.0</v>
       </c>
       <c r="B16" s="21">
@@ -4406,7 +4406,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11">
+      <c r="A17" s="7">
         <v>12.0</v>
       </c>
       <c r="B17" s="21">
@@ -4495,7 +4495,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="11">
+      <c r="A18" s="7">
         <v>13.0</v>
       </c>
       <c r="B18" s="21">
@@ -4584,7 +4584,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="11">
+      <c r="A19" s="7">
         <v>14.0</v>
       </c>
       <c r="B19" s="21">
@@ -4673,7 +4673,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="11">
+      <c r="A20" s="7">
         <v>15.0</v>
       </c>
       <c r="B20" s="21">
@@ -4762,7 +4762,7 @@
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="11">
+      <c r="A21" s="7">
         <v>16.0</v>
       </c>
       <c r="B21" s="21">
@@ -4851,7 +4851,7 @@
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="11">
+      <c r="A22" s="7">
         <v>17.0</v>
       </c>
       <c r="B22" s="21">
@@ -4940,7 +4940,7 @@
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="11">
+      <c r="A23" s="7">
         <v>18.0</v>
       </c>
       <c r="B23" s="21">
@@ -5029,7 +5029,7 @@
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="11">
+      <c r="A24" s="7">
         <v>19.0</v>
       </c>
       <c r="B24" s="21">
@@ -5118,7 +5118,7 @@
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="11">
+      <c r="A25" s="7">
         <v>20.0</v>
       </c>
       <c r="B25" s="21">
@@ -5207,7 +5207,7 @@
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="11">
+      <c r="A26" s="7">
         <v>21.0</v>
       </c>
       <c r="B26" s="21">
@@ -5296,7 +5296,7 @@
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="11">
+      <c r="A27" s="7">
         <v>22.0</v>
       </c>
       <c r="B27" s="21">
@@ -5385,7 +5385,7 @@
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="11">
+      <c r="A28" s="7">
         <v>23.0</v>
       </c>
       <c r="B28" s="21">
@@ -5474,7 +5474,7 @@
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="11">
+      <c r="A29" s="7">
         <v>24.0</v>
       </c>
       <c r="B29" s="21">
@@ -5563,7 +5563,7 @@
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="11">
+      <c r="A30" s="7">
         <v>25.0</v>
       </c>
       <c r="B30" s="21">
@@ -5652,7 +5652,7 @@
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="11">
+      <c r="A31" s="7">
         <v>26.0</v>
       </c>
       <c r="B31" s="21">
@@ -5741,7 +5741,7 @@
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="11">
+      <c r="A32" s="7">
         <v>27.0</v>
       </c>
       <c r="B32" s="21">
@@ -5830,7 +5830,7 @@
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="11">
+      <c r="A33" s="7">
         <v>28.0</v>
       </c>
       <c r="B33" s="21">
@@ -5919,7 +5919,7 @@
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="11">
+      <c r="A34" s="7">
         <v>29.0</v>
       </c>
       <c r="B34" s="21">
@@ -6008,7 +6008,7 @@
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="11">
+      <c r="A35" s="7">
         <v>30.0</v>
       </c>
       <c r="B35" s="21">
@@ -6097,7 +6097,7 @@
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="11">
+      <c r="A36" s="7">
         <v>31.0</v>
       </c>
       <c r="B36" s="21">
@@ -6186,7 +6186,7 @@
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="11">
+      <c r="A37" s="7">
         <v>31.0</v>
       </c>
       <c r="B37" s="21">
@@ -7271,91 +7271,91 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="12">
         <v>1.0</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="11">
         <v>200.0</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="13">
         <v>1000.0</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="13">
         <v>130.0</v>
       </c>
       <c r="N2" s="3"/>
@@ -7364,100 +7364,100 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
-      <c r="T2" s="7"/>
+      <c r="T2" s="10"/>
     </row>
     <row r="3">
-      <c r="A3" s="11"/>
-      <c r="C3" s="12" t="s">
+      <c r="A3" s="7"/>
+      <c r="C3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="V3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="W3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="Y3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="Z3" s="12" t="s">
+      <c r="Z3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AA3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="AB3" s="12" t="s">
+      <c r="AB3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="AC3" s="12" t="s">
+      <c r="AC3" s="14" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="s">
-        <v>0</v>
+      <c r="A4" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="15" t="s">
         <v>77</v>
       </c>
       <c r="D4" s="16" t="s">
@@ -7469,16 +7469,16 @@
       <c r="F4" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="15" t="s">
         <v>82</v>
       </c>
       <c r="I4" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="15" t="s">
         <v>84</v>
       </c>
       <c r="K4" s="16" t="s">
@@ -7499,7 +7499,7 @@
       <c r="P4" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" s="15" t="s">
         <v>91</v>
       </c>
       <c r="R4" s="18" t="s">
@@ -7508,7 +7508,7 @@
       <c r="S4" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="T4" s="14" t="s">
+      <c r="T4" s="15" t="s">
         <v>94</v>
       </c>
       <c r="U4" s="19" t="s">
@@ -7540,7 +7540,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B5" s="21">
@@ -7629,7 +7629,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11">
+      <c r="A6" s="7">
         <v>1.0</v>
       </c>
       <c r="B6" s="21">
@@ -7718,7 +7718,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11">
+      <c r="A7" s="7">
         <v>2.0</v>
       </c>
       <c r="B7" s="21">
@@ -7807,7 +7807,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="11">
+      <c r="A8" s="7">
         <v>3.0</v>
       </c>
       <c r="B8" s="21">
@@ -7896,7 +7896,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11">
+      <c r="A9" s="7">
         <v>4.0</v>
       </c>
       <c r="B9" s="21">
@@ -7985,7 +7985,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="11">
+      <c r="A10" s="7">
         <v>5.0</v>
       </c>
       <c r="B10" s="21">
@@ -8074,7 +8074,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11">
+      <c r="A11" s="7">
         <v>6.0</v>
       </c>
       <c r="B11" s="21">
@@ -8163,7 +8163,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="11">
+      <c r="A12" s="7">
         <v>7.0</v>
       </c>
       <c r="B12" s="21">
@@ -8252,7 +8252,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11">
+      <c r="A13" s="7">
         <v>8.0</v>
       </c>
       <c r="B13" s="21">
@@ -8341,7 +8341,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="11">
+      <c r="A14" s="7">
         <v>9.0</v>
       </c>
       <c r="B14" s="21">
@@ -8430,7 +8430,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11">
+      <c r="A15" s="7">
         <v>10.0</v>
       </c>
       <c r="B15" s="21">
@@ -8519,7 +8519,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="11">
+      <c r="A16" s="7">
         <v>11.0</v>
       </c>
       <c r="B16" s="21">
@@ -8608,7 +8608,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11">
+      <c r="A17" s="7">
         <v>12.0</v>
       </c>
       <c r="B17" s="21">
@@ -8697,7 +8697,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="11">
+      <c r="A18" s="7">
         <v>13.0</v>
       </c>
       <c r="B18" s="21">
@@ -8786,7 +8786,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="11">
+      <c r="A19" s="7">
         <v>14.0</v>
       </c>
       <c r="B19" s="21">
@@ -8875,7 +8875,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="11">
+      <c r="A20" s="7">
         <v>15.0</v>
       </c>
       <c r="B20" s="21">
@@ -8964,7 +8964,7 @@
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="11">
+      <c r="A21" s="7">
         <v>16.0</v>
       </c>
       <c r="B21" s="21">
@@ -9053,7 +9053,7 @@
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="11">
+      <c r="A22" s="7">
         <v>17.0</v>
       </c>
       <c r="B22" s="21">
@@ -9142,7 +9142,7 @@
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="11">
+      <c r="A23" s="7">
         <v>18.0</v>
       </c>
       <c r="B23" s="21">
@@ -9231,7 +9231,7 @@
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="11">
+      <c r="A24" s="7">
         <v>19.0</v>
       </c>
       <c r="B24" s="21">
@@ -9320,7 +9320,7 @@
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="11">
+      <c r="A25" s="7">
         <v>20.0</v>
       </c>
       <c r="B25" s="21">
@@ -9409,7 +9409,7 @@
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="11">
+      <c r="A26" s="7">
         <v>21.0</v>
       </c>
       <c r="B26" s="21">
@@ -9498,7 +9498,7 @@
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="11">
+      <c r="A27" s="7">
         <v>22.0</v>
       </c>
       <c r="B27" s="21">
@@ -9587,7 +9587,7 @@
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="11">
+      <c r="A28" s="7">
         <v>23.0</v>
       </c>
       <c r="B28" s="21">
@@ -9676,7 +9676,7 @@
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="11">
+      <c r="A29" s="7">
         <v>24.0</v>
       </c>
       <c r="B29" s="21">
@@ -9765,7 +9765,7 @@
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="11">
+      <c r="A30" s="7">
         <v>25.0</v>
       </c>
       <c r="B30" s="21">
@@ -9854,7 +9854,7 @@
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="11">
+      <c r="A31" s="7">
         <v>26.0</v>
       </c>
       <c r="B31" s="21">
@@ -9943,7 +9943,7 @@
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="11">
+      <c r="A32" s="7">
         <v>27.0</v>
       </c>
       <c r="B32" s="21">
@@ -10032,7 +10032,7 @@
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="11">
+      <c r="A33" s="7">
         <v>28.0</v>
       </c>
       <c r="B33" s="21">
@@ -10121,7 +10121,7 @@
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="11">
+      <c r="A34" s="7">
         <v>29.0</v>
       </c>
       <c r="B34" s="21">
@@ -10210,7 +10210,7 @@
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="11">
+      <c r="A35" s="7">
         <v>30.0</v>
       </c>
       <c r="B35" s="21">
@@ -10299,7 +10299,7 @@
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="11">
+      <c r="A36" s="7">
         <v>31.0</v>
       </c>
       <c r="B36" s="21">
@@ -10388,7 +10388,7 @@
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="11">
+      <c r="A37" s="7">
         <v>31.0</v>
       </c>
       <c r="B37" s="21">

</xml_diff>